<commit_message>
Added support foe date fields
</commit_message>
<xml_diff>
--- a/parser/test_data/invoices/invoice1.xlsx
+++ b/parser/test_data/invoices/invoice1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">top</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">budget</t>
   </si>
 </sst>
 </file>
@@ -154,6 +160,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="n">
@@ -206,6 +215,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
@@ -239,16 +251,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -269,6 +278,22 @@
       </c>
       <c r="C12" s="1" t="n">
         <v>43104</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>